<commit_message>
Added Disk Usage, added Pytests, moved row count, removed downsampled RAM calculatioon
</commit_message>
<xml_diff>
--- a/docs/TestPlan.xlsx
+++ b/docs/TestPlan.xlsx
@@ -12,7 +12,7 @@
     <sheet name="- Disclaimer -" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Test Case Planning &amp; Execution'!$B$1:$H$32</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Test Case Planning &amp; Execution'!$B$1:$H$26</definedName>
     <definedName function="false" hidden="false" name="_ITEM1" vbProcedure="false">'test case planning &amp; execution'!#ref!</definedName>
     <definedName function="false" hidden="false" name="_ITEM2" vbProcedure="false">'test case planning &amp; execution'!#ref!</definedName>
     <definedName function="false" hidden="false" name="_ITEM3" vbProcedure="false">'test case planning &amp; execution'!#ref!</definedName>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <t xml:space="preserve">TEST CASE PLANNING AND EXECUTION</t>
   </si>
@@ -89,7 +89,19 @@
     <t xml:space="preserve">ADDITIONAL NOTES</t>
   </si>
   <si>
-    <t xml:space="preserve">Downsampling Toggle can be selected for each database type</t>
+    <t xml:space="preserve">Clickhouse Tab option can be selected from the home page menu options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PostgreSQL Tab option can be selected from the home page menu options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TimescaleDB Tab option can be selected from the home page menu options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Home Tab option can be selected from the home page menu options</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Downsampling Toggle can be selected for DB1 – (Clickhouse)</t>
   </si>
   <si>
     <t xml:space="preserve">Test Pass – The downsampling toggles can be selected for each database type</t>
@@ -101,13 +113,7 @@
     <t xml:space="preserve">PASS</t>
   </si>
   <si>
-    <t xml:space="preserve">Increment the Downsample Number Input for each Database type – DB 1 (Postgres)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Increment the Downsample Number Input for each Database type – DB 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Increment the Downsample Number Input for each Database type – DB 3</t>
+    <t xml:space="preserve">Increment the Downsample Number Input for each Database type – DB 1 (Clickhouse)</t>
   </si>
   <si>
     <r>
@@ -118,7 +124,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Check the values of each Database type downsampling radio buttons – DB 1</t>
+      <t xml:space="preserve">Change the start date of each Database type – DB 1 (</t>
     </r>
     <r>
       <rPr>
@@ -127,7 +133,17 @@
         <rFont val="Century Gothic"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> (Postgres)</t>
+      <t xml:space="preserve">Clickhouse</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
     </r>
   </si>
   <si>
@@ -139,7 +155,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Check the values of each Database type downsampling radio buttons -</t>
+      <t xml:space="preserve">Change the end date of each Database type – DB 1 (</t>
     </r>
     <r>
       <rPr>
@@ -148,7 +164,17 @@
         <rFont val="Century Gothic"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve"> DB 2</t>
+      <t xml:space="preserve">Clickhouse</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
     </r>
   </si>
   <si>
@@ -160,7 +186,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Check the values of each Database type downsampling radio buttons </t>
+      <t xml:space="preserve">Change the start time of each Database type – DB 1 (</t>
     </r>
     <r>
       <rPr>
@@ -169,7 +195,17 @@
         <rFont val="Century Gothic"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">– DB 3</t>
+      <t xml:space="preserve">Clickhouse</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
     </r>
   </si>
   <si>
@@ -181,7 +217,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Change the value of each Database type </t>
+      <t xml:space="preserve">Change the end time of each Database type – DB 1 (</t>
     </r>
     <r>
       <rPr>
@@ -190,7 +226,54 @@
         <rFont val="Century Gothic"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">downsampling radio buttons – DB 1 (Postgres)</t>
+      <t xml:space="preserve">Clickhouse</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Submit Button can be selected and data ingressed for each Database type – DB 1 (Clickhouse)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Downsampling Toggle can be selected for DB 2 – (PostgreSQL)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Increment the Downsample Number Input for each Database type – DB 2 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">PostgreSQL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
     </r>
   </si>
   <si>
@@ -202,7 +285,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Change the value of each Database type </t>
+      <t xml:space="preserve">Change the start date of each Database type – DB 2 (</t>
     </r>
     <r>
       <rPr>
@@ -211,7 +294,17 @@
         <rFont val="Century Gothic"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">downsampling radio buttons – DB 2</t>
+      <t xml:space="preserve">PostgreSQL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
     </r>
   </si>
   <si>
@@ -223,7 +316,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Change the value of each Database type </t>
+      <t xml:space="preserve">Change the end date of each Database type – DB 2 (</t>
     </r>
     <r>
       <rPr>
@@ -232,40 +325,7 @@
         <rFont val="Century Gothic"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">downsampling radio buttons – DB 3</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Change the start date of each Database type – DB 1 (Postgres)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Change the start date of each Database type – DB 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Change the start date of each Database type – DB 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Change the end date of each Database type – DB 1 (Postgres)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Change the </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">end</t>
+      <t xml:space="preserve">PostgreSQL</t>
     </r>
     <r>
       <rPr>
@@ -275,7 +335,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> date of each Database type – DB 2</t>
+      <t xml:space="preserve">)</t>
     </r>
   </si>
   <si>
@@ -287,7 +347,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Change the </t>
+      <t xml:space="preserve">Change the start time of each Database type – DB 2 (</t>
     </r>
     <r>
       <rPr>
@@ -296,7 +356,7 @@
         <rFont val="Century Gothic"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">end</t>
+      <t xml:space="preserve">PostgreSQL</t>
     </r>
     <r>
       <rPr>
@@ -306,7 +366,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> date of each Database type – DB 3</t>
+      <t xml:space="preserve">)</t>
     </r>
   </si>
   <si>
@@ -318,7 +378,7 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Change the </t>
+      <t xml:space="preserve">Change the end time of each Database type – DB 2 (</t>
     </r>
     <r>
       <rPr>
@@ -327,7 +387,7 @@
         <rFont val="Century Gothic"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">start</t>
+      <t xml:space="preserve">PostgreSQL</t>
     </r>
     <r>
       <rPr>
@@ -337,23 +397,256 @@
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> time of each Database type – DB 1 (Postgres)</t>
+      <t xml:space="preserve">)</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Change the start time of each Database type – DB 2</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Submit Button can be selected and data ingressed for each Database type – DB 2 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">PostgreSQL</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
   </si>
   <si>
-    <t xml:space="preserve">Change the start time of each Database type – DB 3</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Downsampling Toggle can be selected for DB 3 – (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">TimescaleDB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
   </si>
   <si>
-    <t xml:space="preserve">Change the end time of each Database type – DB 1 (Postgres)</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Increment the Downsample Number Input for each Database type – DB 3 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">TimescaleDB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
   </si>
   <si>
-    <t xml:space="preserve">Change the end time of each Database type – DB 2</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Change the start date of each Database type – DB 3 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">TimescaleDB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
   </si>
   <si>
-    <t xml:space="preserve">Change the end time of each Database type – DB 3</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Change the end date of each Database type – DB 3 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">TimescaleDB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Change the start time of each Database type – DB 3 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">TimescaleDB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Change the end time of each Database type – DB 3 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">TimescaleDB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Submit Button can be selected and data ingressed for each Database type – DB 3 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">TimescaleDB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Any articles, templates, or information provided by Smartsheet on the website are for reference only. While we strive to keep the information up to date and correct, we make no representations or warranties of any kind, express or implied, about the completeness, accuracy, reliability, suitability, or availability with respect to the website or the information, articles, templates, or related graphics contained on the website. Any reliance you place on such information is therefore strictly at your own risk. </t>
@@ -768,12 +1061,12 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="13" fillId="12" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -867,12 +1160,12 @@
     <tabColor rgb="FF8497B0"/>
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:EZ911"/>
+  <dimension ref="A1:EZ914"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1195,61 +1488,53 @@
       <c r="C11" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="26" t="n">
-        <v>45345</v>
-      </c>
-      <c r="E11" s="27" t="s">
-        <v>20</v>
-      </c>
-      <c r="F11" s="27" t="s">
-        <v>21</v>
-      </c>
-      <c r="G11" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="H11" s="27"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="29"/>
+      <c r="H11" s="25"/>
     </row>
     <row r="12" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="23"/>
       <c r="B12" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="C12" s="25" t="s">
-        <v>23</v>
+      <c r="C12" s="30" t="s">
+        <v>20</v>
       </c>
       <c r="D12" s="26"/>
       <c r="E12" s="27"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="27"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="25"/>
     </row>
     <row r="13" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="23"/>
       <c r="B13" s="24" t="n">
         <v>3</v>
       </c>
-      <c r="C13" s="25" t="s">
-        <v>24</v>
+      <c r="C13" s="30" t="s">
+        <v>21</v>
       </c>
       <c r="D13" s="26"/>
       <c r="E13" s="27"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="27"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="25"/>
     </row>
     <row r="14" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="23"/>
       <c r="B14" s="24" t="n">
         <v>4</v>
       </c>
-      <c r="C14" s="25" t="s">
-        <v>25</v>
+      <c r="C14" s="30" t="s">
+        <v>22</v>
       </c>
       <c r="D14" s="26"/>
       <c r="E14" s="27"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="27"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="29"/>
+      <c r="H14" s="25"/>
     </row>
     <row r="15" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="23"/>
@@ -1257,13 +1542,21 @@
         <v>5</v>
       </c>
       <c r="C15" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="26" t="n">
+        <v>45345</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="29" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="26"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="29"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="27"/>
+      <c r="H15" s="25"/>
     </row>
     <row r="16" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="23"/>
@@ -1275,9 +1568,9 @@
       </c>
       <c r="D16" s="26"/>
       <c r="E16" s="27"/>
-      <c r="F16" s="29"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="27"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="29"/>
+      <c r="H16" s="25"/>
     </row>
     <row r="17" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="23"/>
@@ -1289,9 +1582,9 @@
       </c>
       <c r="D17" s="26"/>
       <c r="E17" s="27"/>
-      <c r="F17" s="29"/>
-      <c r="G17" s="28"/>
-      <c r="H17" s="27"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="25"/>
     </row>
     <row r="18" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="23"/>
@@ -1303,9 +1596,9 @@
       </c>
       <c r="D18" s="26"/>
       <c r="E18" s="27"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="27"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="29"/>
+      <c r="H18" s="25"/>
     </row>
     <row r="19" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="23"/>
@@ -1317,9 +1610,9 @@
       </c>
       <c r="D19" s="26"/>
       <c r="E19" s="27"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="27"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="29"/>
+      <c r="H19" s="25"/>
     </row>
     <row r="20" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="23"/>
@@ -1331,9 +1624,9 @@
       </c>
       <c r="D20" s="26"/>
       <c r="E20" s="27"/>
-      <c r="F20" s="29"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="27"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="25"/>
     </row>
     <row r="21" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="23"/>
@@ -1345,9 +1638,9 @@
       </c>
       <c r="D21" s="26"/>
       <c r="E21" s="27"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="27"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="25"/>
     </row>
     <row r="22" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="23"/>
@@ -1359,9 +1652,9 @@
       </c>
       <c r="D22" s="26"/>
       <c r="E22" s="27"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="28"/>
-      <c r="H22" s="27"/>
+      <c r="F22" s="28"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="25"/>
     </row>
     <row r="23" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="23"/>
@@ -1373,9 +1666,9 @@
       </c>
       <c r="D23" s="26"/>
       <c r="E23" s="27"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="27"/>
+      <c r="F23" s="28"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="25"/>
     </row>
     <row r="24" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="23"/>
@@ -1387,9 +1680,9 @@
       </c>
       <c r="D24" s="26"/>
       <c r="E24" s="27"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="28"/>
-      <c r="H24" s="27"/>
+      <c r="F24" s="28"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="25"/>
     </row>
     <row r="25" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="23"/>
@@ -1401,9 +1694,9 @@
       </c>
       <c r="D25" s="26"/>
       <c r="E25" s="27"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="27"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="25"/>
     </row>
     <row r="26" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="23"/>
@@ -1415,9 +1708,9 @@
       </c>
       <c r="D26" s="26"/>
       <c r="E26" s="27"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="27"/>
+      <c r="F26" s="28"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="25"/>
     </row>
     <row r="27" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="23"/>
@@ -1429,259 +1722,123 @@
       </c>
       <c r="D27" s="26"/>
       <c r="E27" s="27"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="27"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="25"/>
     </row>
     <row r="28" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="23"/>
       <c r="B28" s="24" t="n">
         <v>18</v>
       </c>
-      <c r="C28" s="30" t="s">
+      <c r="C28" s="25" t="s">
         <v>39</v>
       </c>
       <c r="D28" s="26"/>
       <c r="E28" s="27"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="27"/>
+      <c r="F28" s="28"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="25"/>
     </row>
     <row r="29" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="23"/>
       <c r="B29" s="24" t="n">
         <v>19</v>
       </c>
-      <c r="C29" s="30" t="s">
+      <c r="C29" s="25" t="s">
         <v>40</v>
       </c>
       <c r="D29" s="26"/>
       <c r="E29" s="27"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="27"/>
+      <c r="F29" s="28"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="25"/>
     </row>
     <row r="30" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="23"/>
       <c r="B30" s="24" t="n">
         <v>20</v>
       </c>
-      <c r="C30" s="30" t="s">
+      <c r="C30" s="25" t="s">
         <v>41</v>
       </c>
       <c r="D30" s="26"/>
       <c r="E30" s="27"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="28"/>
-      <c r="H30" s="27"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="25"/>
     </row>
     <row r="31" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="23"/>
       <c r="B31" s="24" t="n">
         <v>21</v>
       </c>
-      <c r="C31" s="30" t="s">
+      <c r="C31" s="25" t="s">
         <v>42</v>
       </c>
       <c r="D31" s="26"/>
       <c r="E31" s="27"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="28"/>
-      <c r="H31" s="27"/>
+      <c r="F31" s="28"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="25"/>
     </row>
     <row r="32" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="23"/>
       <c r="B32" s="24" t="n">
         <v>22</v>
       </c>
-      <c r="C32" s="30" t="s">
+      <c r="C32" s="25" t="s">
         <v>43</v>
       </c>
       <c r="D32" s="26"/>
       <c r="E32" s="27"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="28"/>
-      <c r="H32" s="27"/>
-    </row>
-    <row r="33" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="12"/>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
-      <c r="H33" s="12"/>
-    </row>
-    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="12"/>
-      <c r="B34" s="12"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="12"/>
-      <c r="E34" s="12"/>
-      <c r="F34" s="12"/>
-      <c r="G34" s="12"/>
-      <c r="H34" s="12"/>
-    </row>
-    <row r="35" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="12"/>
-      <c r="B35" s="12"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="12"/>
-      <c r="E35" s="12"/>
-      <c r="F35" s="12"/>
-      <c r="G35" s="12"/>
-      <c r="H35" s="12"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
-      <c r="N35" s="1"/>
-      <c r="O35" s="1"/>
-      <c r="P35" s="1"/>
-      <c r="Q35" s="1"/>
-      <c r="R35" s="1"/>
-      <c r="S35" s="1"/>
-      <c r="T35" s="1"/>
-      <c r="U35" s="1"/>
-      <c r="V35" s="1"/>
-      <c r="W35" s="1"/>
-      <c r="X35" s="1"/>
-      <c r="Y35" s="1"/>
-      <c r="Z35" s="1"/>
-      <c r="AA35" s="1"/>
-      <c r="AB35" s="1"/>
-      <c r="AC35" s="1"/>
-      <c r="AD35" s="1"/>
-      <c r="AE35" s="1"/>
-      <c r="AF35" s="1"/>
-      <c r="AG35" s="1"/>
-      <c r="AH35" s="1"/>
-      <c r="AI35" s="1"/>
-      <c r="AJ35" s="1"/>
-      <c r="AK35" s="1"/>
-      <c r="AL35" s="1"/>
-      <c r="AM35" s="1"/>
-      <c r="AN35" s="1"/>
-      <c r="AO35" s="1"/>
-      <c r="AP35" s="1"/>
-      <c r="AQ35" s="1"/>
-      <c r="AR35" s="1"/>
-      <c r="AS35" s="1"/>
-      <c r="AT35" s="1"/>
-      <c r="AU35" s="1"/>
-      <c r="AV35" s="1"/>
-      <c r="AW35" s="1"/>
-      <c r="AX35" s="1"/>
-      <c r="AY35" s="1"/>
-      <c r="AZ35" s="1"/>
-      <c r="BA35" s="1"/>
-      <c r="BB35" s="1"/>
-      <c r="BC35" s="1"/>
-      <c r="BD35" s="1"/>
-      <c r="BE35" s="1"/>
-      <c r="BF35" s="1"/>
-      <c r="BG35" s="1"/>
-      <c r="BH35" s="1"/>
-      <c r="BI35" s="1"/>
-      <c r="BJ35" s="1"/>
-      <c r="BK35" s="1"/>
-      <c r="BL35" s="1"/>
-      <c r="BM35" s="1"/>
-      <c r="BN35" s="1"/>
-      <c r="BO35" s="1"/>
-      <c r="BP35" s="1"/>
-      <c r="BQ35" s="1"/>
-      <c r="BR35" s="1"/>
-      <c r="BS35" s="1"/>
-      <c r="BT35" s="1"/>
-      <c r="BU35" s="1"/>
-      <c r="BV35" s="1"/>
-      <c r="BW35" s="1"/>
-      <c r="BX35" s="1"/>
-      <c r="BY35" s="1"/>
-      <c r="BZ35" s="1"/>
-      <c r="CA35" s="1"/>
-      <c r="CB35" s="1"/>
-      <c r="CC35" s="1"/>
-      <c r="CD35" s="1"/>
-      <c r="CE35" s="1"/>
-      <c r="CF35" s="1"/>
-      <c r="CG35" s="1"/>
-      <c r="CH35" s="1"/>
-      <c r="CI35" s="1"/>
-      <c r="CJ35" s="1"/>
-      <c r="CK35" s="1"/>
-      <c r="CL35" s="1"/>
-      <c r="CM35" s="1"/>
-      <c r="CN35" s="1"/>
-      <c r="CO35" s="1"/>
-      <c r="CP35" s="1"/>
-      <c r="CQ35" s="1"/>
-      <c r="CR35" s="1"/>
-      <c r="CS35" s="1"/>
-      <c r="CT35" s="1"/>
-      <c r="CU35" s="1"/>
-      <c r="CV35" s="1"/>
-      <c r="CW35" s="1"/>
-      <c r="CX35" s="1"/>
-      <c r="CY35" s="1"/>
-      <c r="CZ35" s="1"/>
-      <c r="DA35" s="1"/>
-      <c r="DB35" s="1"/>
-      <c r="DC35" s="1"/>
-      <c r="DD35" s="1"/>
-      <c r="DE35" s="1"/>
-      <c r="DF35" s="1"/>
-      <c r="DG35" s="1"/>
-      <c r="DH35" s="1"/>
-      <c r="DI35" s="1"/>
-      <c r="DJ35" s="1"/>
-      <c r="DK35" s="1"/>
-      <c r="DL35" s="1"/>
-      <c r="DM35" s="1"/>
-      <c r="DN35" s="1"/>
-      <c r="DO35" s="1"/>
-      <c r="DP35" s="1"/>
-      <c r="DQ35" s="1"/>
-      <c r="DR35" s="1"/>
-      <c r="DS35" s="1"/>
-      <c r="DT35" s="1"/>
-      <c r="DU35" s="1"/>
-      <c r="DV35" s="1"/>
-      <c r="DW35" s="1"/>
-      <c r="DX35" s="1"/>
-      <c r="DY35" s="1"/>
-      <c r="DZ35" s="1"/>
-      <c r="EA35" s="1"/>
-      <c r="EB35" s="1"/>
-      <c r="EC35" s="1"/>
-      <c r="ED35" s="1"/>
-      <c r="EE35" s="1"/>
-      <c r="EF35" s="1"/>
-      <c r="EG35" s="1"/>
-      <c r="EH35" s="1"/>
-      <c r="EI35" s="1"/>
-      <c r="EJ35" s="1"/>
-      <c r="EK35" s="1"/>
-      <c r="EL35" s="1"/>
-      <c r="EM35" s="1"/>
-      <c r="EN35" s="1"/>
-      <c r="EO35" s="1"/>
-      <c r="EP35" s="1"/>
-      <c r="EQ35" s="1"/>
-      <c r="ER35" s="1"/>
-      <c r="ES35" s="1"/>
-      <c r="ET35" s="1"/>
-      <c r="EU35" s="1"/>
-      <c r="EV35" s="1"/>
-      <c r="EW35" s="1"/>
-      <c r="EX35" s="1"/>
-      <c r="EY35" s="1"/>
-      <c r="EZ35" s="1"/>
-    </row>
-    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F32" s="28"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="25"/>
+    </row>
+    <row r="33" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="23"/>
+      <c r="B33" s="24" t="n">
+        <v>23</v>
+      </c>
+      <c r="C33" s="25" t="s">
+        <v>44</v>
+      </c>
+      <c r="D33" s="26"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="25"/>
+    </row>
+    <row r="34" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="23"/>
+      <c r="B34" s="24" t="n">
+        <v>24</v>
+      </c>
+      <c r="C34" s="25" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="26"/>
+      <c r="E34" s="27"/>
+      <c r="F34" s="28"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="25"/>
+    </row>
+    <row r="35" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="23"/>
+      <c r="B35" s="24" t="n">
+        <v>25</v>
+      </c>
+      <c r="C35" s="25" t="s">
+        <v>46</v>
+      </c>
+      <c r="D35" s="26"/>
+      <c r="E35" s="27"/>
+      <c r="F35" s="28"/>
+      <c r="G35" s="29"/>
+      <c r="H35" s="25"/>
+    </row>
+    <row r="36" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="12"/>
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
@@ -1761,7 +1918,7 @@
       <c r="G43" s="12"/>
       <c r="H43" s="12"/>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="12"/>
       <c r="B44" s="12"/>
       <c r="C44" s="12"/>
@@ -1770,6 +1927,154 @@
       <c r="F44" s="12"/>
       <c r="G44" s="12"/>
       <c r="H44" s="12"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+      <c r="L44" s="1"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1"/>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="1"/>
+      <c r="R44" s="1"/>
+      <c r="S44" s="1"/>
+      <c r="T44" s="1"/>
+      <c r="U44" s="1"/>
+      <c r="V44" s="1"/>
+      <c r="W44" s="1"/>
+      <c r="X44" s="1"/>
+      <c r="Y44" s="1"/>
+      <c r="Z44" s="1"/>
+      <c r="AA44" s="1"/>
+      <c r="AB44" s="1"/>
+      <c r="AC44" s="1"/>
+      <c r="AD44" s="1"/>
+      <c r="AE44" s="1"/>
+      <c r="AF44" s="1"/>
+      <c r="AG44" s="1"/>
+      <c r="AH44" s="1"/>
+      <c r="AI44" s="1"/>
+      <c r="AJ44" s="1"/>
+      <c r="AK44" s="1"/>
+      <c r="AL44" s="1"/>
+      <c r="AM44" s="1"/>
+      <c r="AN44" s="1"/>
+      <c r="AO44" s="1"/>
+      <c r="AP44" s="1"/>
+      <c r="AQ44" s="1"/>
+      <c r="AR44" s="1"/>
+      <c r="AS44" s="1"/>
+      <c r="AT44" s="1"/>
+      <c r="AU44" s="1"/>
+      <c r="AV44" s="1"/>
+      <c r="AW44" s="1"/>
+      <c r="AX44" s="1"/>
+      <c r="AY44" s="1"/>
+      <c r="AZ44" s="1"/>
+      <c r="BA44" s="1"/>
+      <c r="BB44" s="1"/>
+      <c r="BC44" s="1"/>
+      <c r="BD44" s="1"/>
+      <c r="BE44" s="1"/>
+      <c r="BF44" s="1"/>
+      <c r="BG44" s="1"/>
+      <c r="BH44" s="1"/>
+      <c r="BI44" s="1"/>
+      <c r="BJ44" s="1"/>
+      <c r="BK44" s="1"/>
+      <c r="BL44" s="1"/>
+      <c r="BM44" s="1"/>
+      <c r="BN44" s="1"/>
+      <c r="BO44" s="1"/>
+      <c r="BP44" s="1"/>
+      <c r="BQ44" s="1"/>
+      <c r="BR44" s="1"/>
+      <c r="BS44" s="1"/>
+      <c r="BT44" s="1"/>
+      <c r="BU44" s="1"/>
+      <c r="BV44" s="1"/>
+      <c r="BW44" s="1"/>
+      <c r="BX44" s="1"/>
+      <c r="BY44" s="1"/>
+      <c r="BZ44" s="1"/>
+      <c r="CA44" s="1"/>
+      <c r="CB44" s="1"/>
+      <c r="CC44" s="1"/>
+      <c r="CD44" s="1"/>
+      <c r="CE44" s="1"/>
+      <c r="CF44" s="1"/>
+      <c r="CG44" s="1"/>
+      <c r="CH44" s="1"/>
+      <c r="CI44" s="1"/>
+      <c r="CJ44" s="1"/>
+      <c r="CK44" s="1"/>
+      <c r="CL44" s="1"/>
+      <c r="CM44" s="1"/>
+      <c r="CN44" s="1"/>
+      <c r="CO44" s="1"/>
+      <c r="CP44" s="1"/>
+      <c r="CQ44" s="1"/>
+      <c r="CR44" s="1"/>
+      <c r="CS44" s="1"/>
+      <c r="CT44" s="1"/>
+      <c r="CU44" s="1"/>
+      <c r="CV44" s="1"/>
+      <c r="CW44" s="1"/>
+      <c r="CX44" s="1"/>
+      <c r="CY44" s="1"/>
+      <c r="CZ44" s="1"/>
+      <c r="DA44" s="1"/>
+      <c r="DB44" s="1"/>
+      <c r="DC44" s="1"/>
+      <c r="DD44" s="1"/>
+      <c r="DE44" s="1"/>
+      <c r="DF44" s="1"/>
+      <c r="DG44" s="1"/>
+      <c r="DH44" s="1"/>
+      <c r="DI44" s="1"/>
+      <c r="DJ44" s="1"/>
+      <c r="DK44" s="1"/>
+      <c r="DL44" s="1"/>
+      <c r="DM44" s="1"/>
+      <c r="DN44" s="1"/>
+      <c r="DO44" s="1"/>
+      <c r="DP44" s="1"/>
+      <c r="DQ44" s="1"/>
+      <c r="DR44" s="1"/>
+      <c r="DS44" s="1"/>
+      <c r="DT44" s="1"/>
+      <c r="DU44" s="1"/>
+      <c r="DV44" s="1"/>
+      <c r="DW44" s="1"/>
+      <c r="DX44" s="1"/>
+      <c r="DY44" s="1"/>
+      <c r="DZ44" s="1"/>
+      <c r="EA44" s="1"/>
+      <c r="EB44" s="1"/>
+      <c r="EC44" s="1"/>
+      <c r="ED44" s="1"/>
+      <c r="EE44" s="1"/>
+      <c r="EF44" s="1"/>
+      <c r="EG44" s="1"/>
+      <c r="EH44" s="1"/>
+      <c r="EI44" s="1"/>
+      <c r="EJ44" s="1"/>
+      <c r="EK44" s="1"/>
+      <c r="EL44" s="1"/>
+      <c r="EM44" s="1"/>
+      <c r="EN44" s="1"/>
+      <c r="EO44" s="1"/>
+      <c r="EP44" s="1"/>
+      <c r="EQ44" s="1"/>
+      <c r="ER44" s="1"/>
+      <c r="ES44" s="1"/>
+      <c r="ET44" s="1"/>
+      <c r="EU44" s="1"/>
+      <c r="EV44" s="1"/>
+      <c r="EW44" s="1"/>
+      <c r="EX44" s="1"/>
+      <c r="EY44" s="1"/>
+      <c r="EZ44" s="1"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="12"/>
@@ -1899,7 +2204,7 @@
       <c r="E57" s="12"/>
       <c r="F57" s="12"/>
       <c r="G57" s="12"/>
-      <c r="EZ57" s="8"/>
+      <c r="H57" s="12"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="12"/>
@@ -1909,7 +2214,7 @@
       <c r="E58" s="12"/>
       <c r="F58" s="12"/>
       <c r="G58" s="12"/>
-      <c r="EZ58" s="8"/>
+      <c r="H58" s="12"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="12"/>
@@ -1919,7 +2224,7 @@
       <c r="E59" s="12"/>
       <c r="F59" s="12"/>
       <c r="G59" s="12"/>
-      <c r="EZ59" s="8"/>
+      <c r="H59" s="12"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="12"/>
@@ -1939,7 +2244,7 @@
       <c r="E61" s="12"/>
       <c r="F61" s="12"/>
       <c r="G61" s="12"/>
-      <c r="H61" s="12"/>
+      <c r="EZ61" s="8"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="12"/>
@@ -1949,7 +2254,7 @@
       <c r="E62" s="12"/>
       <c r="F62" s="12"/>
       <c r="G62" s="12"/>
-      <c r="H62" s="12"/>
+      <c r="EZ62" s="8"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="12"/>
@@ -1959,7 +2264,7 @@
       <c r="E63" s="12"/>
       <c r="F63" s="12"/>
       <c r="G63" s="12"/>
-      <c r="H63" s="12"/>
+      <c r="EZ63" s="8"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="12"/>
@@ -10433,6 +10738,36 @@
     </row>
     <row r="911" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A911" s="12"/>
+      <c r="B911" s="12"/>
+      <c r="C911" s="12"/>
+      <c r="D911" s="12"/>
+      <c r="E911" s="12"/>
+      <c r="F911" s="12"/>
+      <c r="G911" s="12"/>
+      <c r="H911" s="12"/>
+    </row>
+    <row r="912" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A912" s="12"/>
+      <c r="B912" s="12"/>
+      <c r="C912" s="12"/>
+      <c r="D912" s="12"/>
+      <c r="E912" s="12"/>
+      <c r="F912" s="12"/>
+      <c r="G912" s="12"/>
+      <c r="H912" s="12"/>
+    </row>
+    <row r="913" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A913" s="12"/>
+      <c r="B913" s="12"/>
+      <c r="C913" s="12"/>
+      <c r="D913" s="12"/>
+      <c r="E913" s="12"/>
+      <c r="F913" s="12"/>
+      <c r="G913" s="12"/>
+      <c r="H913" s="12"/>
+    </row>
+    <row r="914" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A914" s="12"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
@@ -10467,7 +10802,7 @@
     <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="105" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="32" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test updates, updated to use multi page
</commit_message>
<xml_diff>
--- a/docs/TestPlan.xlsx
+++ b/docs/TestPlan.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="60">
   <si>
     <t xml:space="preserve">TEST CASE PLANNING AND EXECUTION</t>
   </si>
@@ -89,16 +89,13 @@
     <t xml:space="preserve">ADDITIONAL NOTES</t>
   </si>
   <si>
-    <t xml:space="preserve">Clickhouse Tab option can be selected from the home page menu options</t>
+    <t xml:space="preserve">A test to check the Home Page opens</t>
   </si>
   <si>
-    <t xml:space="preserve">PostgreSQL Tab option can be selected from the home page menu options</t>
+    <t xml:space="preserve">Test Pass- The home page can be opened</t>
   </si>
   <si>
-    <t xml:space="preserve">TimescaleDB Tab option can be selected from the home page menu options</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Home Tab option can be selected from the home page menu options</t>
+    <t xml:space="preserve">PASS</t>
   </si>
   <si>
     <t xml:space="preserve">Downsampling Toggle can be selected for DB1 – (Clickhouse)</t>
@@ -107,546 +104,127 @@
     <t xml:space="preserve">Test Pass – The downsampling toggles can be selected for each database type</t>
   </si>
   <si>
-    <t xml:space="preserve">Test Passed – The downsampling toggles can be selected for each database type</t>
+    <t xml:space="preserve">Increment the Downsample Number Input for each Database type – DB 1 (Clickhouse)</t>
   </si>
   <si>
-    <t xml:space="preserve">PASS</t>
+    <t xml:space="preserve">Test Pass – The downsampling value is incremented by 1 to a value of 6 (min is 5)</t>
   </si>
   <si>
-    <t xml:space="preserve">Increment the Downsample Number Input for each Database type – DB 1 (Clickhouse)</t>
+    <t xml:space="preserve">Set the Downsample Number Input for each Database type – DB 1 (Clickhouse)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Pass – The downsampling value is set to a value of 5000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change the start date of each Database type – DB 1 (Clickhouse)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Pass – The start date can be changed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change the end date of each Database type – DB 1 (Clickhouse)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Pass – The end date can be changed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change the start time of each Database type – DB 1 (Clickhouse)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Pass – The start time can be changed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change the end time of each Database type – DB 1 (Clickhouse)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Pass – The end time can be changed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Submit Button can be selected and data ingressed for each Database type – DB 1 (Clickhouse)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Pass – The submit button can be selected and the data is imported</t>
   </si>
   <si>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Century Gothic"/>
         <family val="1"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Change the start date of each Database type – DB 1 (</t>
+      <t xml:space="preserve">Test Expected Fail (Due to pytest timeout) -</t>
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Century Gothic"/>
         <family val="1"/>
       </rPr>
-      <t xml:space="preserve">Clickhouse</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
+      <t xml:space="preserve"> The submit button can be selected and the data is imported</t>
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Change the end date of each Database type – DB 1 (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">Clickhouse</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Change the start time of each Database type – DB 1 (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">Clickhouse</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Change the end time of each Database type – DB 1 (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">Clickhouse</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Submit Button can be selected and data ingressed for each Database type – DB 1 (Clickhouse)</t>
+    <t xml:space="preserve">Test times out after 3 seconds, set as XFAIL when it times out passes as it shows data is being imported</t>
   </si>
   <si>
     <t xml:space="preserve">Downsampling Toggle can be selected for DB 2 – (PostgreSQL)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Increment the Downsample Number Input for each Database type – DB 2 (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">PostgreSQL</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
+    <t xml:space="preserve">Increment the Downsample Number Input for each Database type – DB 2 (PostgreSQL)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Change the start date of each Database type – DB 2 (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">PostgreSQL</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
+    <t xml:space="preserve">Set the Downsample Number Input for each Database type – DB 2 (PostgreSQL)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Change the end date of each Database type – DB 2 (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">PostgreSQL</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
+    <t xml:space="preserve">Change the start date of each Database type – DB 2 (PostgreSQL)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Change the start time of each Database type – DB 2 (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">PostgreSQL</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
+    <t xml:space="preserve">Change the end date of each Database type – DB 2 (PostgreSQL)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Change the end time of each Database type – DB 2 (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">PostgreSQL</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
+    <t xml:space="preserve">Change the start time of each Database type – DB 2 (PostgreSQL)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Submit Button can be selected and data ingressed for each Database type – DB 2 (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">PostgreSQL</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
+    <t xml:space="preserve">Change the end time of each Database type – DB 2 (PostgreSQL)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Downsampling Toggle can be selected for DB 3 – (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">TimescaleDB</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
+    <t xml:space="preserve">Submit Button can be selected and data ingressed for each Database type – DB 2 (PostgreSQL)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Increment the Downsample Number Input for each Database type – DB 3 (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">TimescaleDB</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
+    <t xml:space="preserve">Downsampling Toggle can be selected for DB 3 – (TimescaleDB)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Change the start date of each Database type – DB 3 (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">TimescaleDB</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
+    <t xml:space="preserve">Increment the Downsample Number Input for each Database type – DB 3 (TimescaleDB)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Change the end date of each Database type – DB 3 (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">TimescaleDB</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
+    <t xml:space="preserve">Set the Downsample Number Input for each Database type – DB 3 (TimescaleDB)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Change the start time of each Database type – DB 3 (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">TimescaleDB</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
+    <t xml:space="preserve">Change the start date of each Database type – DB 3 (TimescaleDB)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Change the end time of each Database type – DB 3 (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">TimescaleDB</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
+    <t xml:space="preserve">Change the end date of each Database type – DB 3 (TimescaleDB)</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Submit Button can be selected and data ingressed for each Database type – DB 3 (</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve">TimescaleDB</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">)</t>
-    </r>
+    <t xml:space="preserve">Change the start time of each Database type – DB 3 (TimescaleDB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change the end time of each Database type – DB 3 (TimescaleDB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Submit Button can be selected and data ingressed for each Database type – DB 3 (TimescaleDB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All values can be edited and stay the selected values when the submit button is selected – DB 1 (Clickhouse)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All values can be edited and stay the selected values when the submit button is selected – DB 2 (PostgreSQL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All values can be edited and stay the selected values when the submit button is selected – DB 1 (TimescaleDB)</t>
   </si>
   <si>
     <t xml:space="preserve">Any articles, templates, or information provided by Smartsheet on the website are for reference only. While we strive to keep the information up to date and correct, we make no representations or warranties of any kind, express or implied, about the completeness, accuracy, reliability, suitability, or availability with respect to the website or the information, articles, templates, or related graphics contained on the website. Any reliance you place on such information is therefore strictly at your own risk. </t>
@@ -660,7 +238,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -747,6 +325,12 @@
       <name val="Century Gothic"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Century Gothic"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -948,7 +532,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1061,7 +645,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1069,7 +653,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="12" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="12" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1077,7 +669,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="6" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="6" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="2" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1160,12 +752,12 @@
     <tabColor rgb="FF8497B0"/>
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:EZ914"/>
+  <dimension ref="A1:EZ917"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
+      <selection pane="bottomLeft" activeCell="H27" activeCellId="0" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1488,10 +1080,18 @@
       <c r="C11" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="27"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="29"/>
+      <c r="D11" s="26" t="n">
+        <v>45375</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="29" t="s">
+        <v>21</v>
+      </c>
       <c r="H11" s="25"/>
     </row>
     <row r="12" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1499,13 +1099,21 @@
       <c r="B12" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="C12" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="28"/>
-      <c r="G12" s="29"/>
+      <c r="C12" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="26" t="n">
+        <v>45375</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="29" t="s">
+        <v>21</v>
+      </c>
       <c r="H12" s="25"/>
     </row>
     <row r="13" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1513,13 +1121,21 @@
       <c r="B13" s="24" t="n">
         <v>3</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="26" t="n">
+        <v>45375</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="26"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="29"/>
       <c r="H13" s="25"/>
     </row>
     <row r="14" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1527,13 +1143,21 @@
       <c r="B14" s="24" t="n">
         <v>4</v>
       </c>
-      <c r="C14" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="26"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="29"/>
+      <c r="C14" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="D14" s="26" t="n">
+        <v>45375</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>27</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="29" t="s">
+        <v>21</v>
+      </c>
       <c r="H14" s="25"/>
     </row>
     <row r="15" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1542,19 +1166,19 @@
         <v>5</v>
       </c>
       <c r="C15" s="25" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D15" s="26" t="n">
-        <v>45345</v>
-      </c>
-      <c r="E15" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="F15" s="27" t="s">
-        <v>25</v>
+        <v>45375</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>29</v>
+      </c>
+      <c r="F15" s="28" t="s">
+        <v>29</v>
       </c>
       <c r="G15" s="29" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="H15" s="25"/>
     </row>
@@ -1564,12 +1188,20 @@
         <v>6</v>
       </c>
       <c r="C16" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="26"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="29"/>
+        <v>30</v>
+      </c>
+      <c r="D16" s="26" t="n">
+        <v>45375</v>
+      </c>
+      <c r="E16" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="G16" s="29" t="s">
+        <v>21</v>
+      </c>
       <c r="H16" s="25"/>
     </row>
     <row r="17" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1578,12 +1210,20 @@
         <v>7</v>
       </c>
       <c r="C17" s="25" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="26"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="29"/>
+        <v>32</v>
+      </c>
+      <c r="D17" s="26" t="n">
+        <v>45375</v>
+      </c>
+      <c r="E17" s="30" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="G17" s="29" t="s">
+        <v>21</v>
+      </c>
       <c r="H17" s="25"/>
     </row>
     <row r="18" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1592,12 +1232,20 @@
         <v>8</v>
       </c>
       <c r="C18" s="25" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="26"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="29"/>
+        <v>34</v>
+      </c>
+      <c r="D18" s="26" t="n">
+        <v>45375</v>
+      </c>
+      <c r="E18" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" s="29" t="s">
+        <v>21</v>
+      </c>
       <c r="H18" s="25"/>
     </row>
     <row r="19" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1606,13 +1254,23 @@
         <v>9</v>
       </c>
       <c r="C19" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="26"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="25"/>
+        <v>36</v>
+      </c>
+      <c r="D19" s="26" t="n">
+        <v>45375</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="F19" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" s="29" t="s">
+        <v>21</v>
+      </c>
+      <c r="H19" s="25" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="23"/>
@@ -1620,11 +1278,11 @@
         <v>10</v>
       </c>
       <c r="C20" s="25" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D20" s="26"/>
       <c r="E20" s="27"/>
-      <c r="F20" s="28"/>
+      <c r="F20" s="31"/>
       <c r="G20" s="29"/>
       <c r="H20" s="25"/>
     </row>
@@ -1634,11 +1292,11 @@
         <v>11</v>
       </c>
       <c r="C21" s="25" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="D21" s="26"/>
       <c r="E21" s="27"/>
-      <c r="F21" s="28"/>
+      <c r="F21" s="31"/>
       <c r="G21" s="29"/>
       <c r="H21" s="25"/>
     </row>
@@ -1648,11 +1306,11 @@
         <v>12</v>
       </c>
       <c r="C22" s="25" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="D22" s="26"/>
       <c r="E22" s="27"/>
-      <c r="F22" s="28"/>
+      <c r="F22" s="31"/>
       <c r="G22" s="29"/>
       <c r="H22" s="25"/>
     </row>
@@ -1662,11 +1320,11 @@
         <v>13</v>
       </c>
       <c r="C23" s="25" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D23" s="26"/>
       <c r="E23" s="27"/>
-      <c r="F23" s="28"/>
+      <c r="F23" s="31"/>
       <c r="G23" s="29"/>
       <c r="H23" s="25"/>
     </row>
@@ -1676,11 +1334,11 @@
         <v>14</v>
       </c>
       <c r="C24" s="25" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="D24" s="26"/>
       <c r="E24" s="27"/>
-      <c r="F24" s="28"/>
+      <c r="F24" s="31"/>
       <c r="G24" s="29"/>
       <c r="H24" s="25"/>
     </row>
@@ -1690,11 +1348,11 @@
         <v>15</v>
       </c>
       <c r="C25" s="25" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="D25" s="26"/>
       <c r="E25" s="27"/>
-      <c r="F25" s="28"/>
+      <c r="F25" s="31"/>
       <c r="G25" s="29"/>
       <c r="H25" s="25"/>
     </row>
@@ -1704,11 +1362,11 @@
         <v>16</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="D26" s="26"/>
       <c r="E26" s="27"/>
-      <c r="F26" s="28"/>
+      <c r="F26" s="31"/>
       <c r="G26" s="29"/>
       <c r="H26" s="25"/>
     </row>
@@ -1718,11 +1376,11 @@
         <v>17</v>
       </c>
       <c r="C27" s="25" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="D27" s="26"/>
       <c r="E27" s="27"/>
-      <c r="F27" s="28"/>
+      <c r="F27" s="31"/>
       <c r="G27" s="29"/>
       <c r="H27" s="25"/>
     </row>
@@ -1732,11 +1390,11 @@
         <v>18</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="D28" s="26"/>
       <c r="E28" s="27"/>
-      <c r="F28" s="28"/>
+      <c r="F28" s="31"/>
       <c r="G28" s="29"/>
       <c r="H28" s="25"/>
     </row>
@@ -1746,11 +1404,11 @@
         <v>19</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="D29" s="26"/>
       <c r="E29" s="27"/>
-      <c r="F29" s="28"/>
+      <c r="F29" s="31"/>
       <c r="G29" s="29"/>
       <c r="H29" s="25"/>
     </row>
@@ -1760,11 +1418,11 @@
         <v>20</v>
       </c>
       <c r="C30" s="25" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D30" s="26"/>
       <c r="E30" s="27"/>
-      <c r="F30" s="28"/>
+      <c r="F30" s="31"/>
       <c r="G30" s="29"/>
       <c r="H30" s="25"/>
     </row>
@@ -1774,11 +1432,11 @@
         <v>21</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="D31" s="26"/>
       <c r="E31" s="27"/>
-      <c r="F31" s="28"/>
+      <c r="F31" s="31"/>
       <c r="G31" s="29"/>
       <c r="H31" s="25"/>
     </row>
@@ -1788,11 +1446,11 @@
         <v>22</v>
       </c>
       <c r="C32" s="25" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="D32" s="26"/>
       <c r="E32" s="27"/>
-      <c r="F32" s="28"/>
+      <c r="F32" s="31"/>
       <c r="G32" s="29"/>
       <c r="H32" s="25"/>
     </row>
@@ -1802,11 +1460,11 @@
         <v>23</v>
       </c>
       <c r="C33" s="25" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="D33" s="26"/>
       <c r="E33" s="27"/>
-      <c r="F33" s="28"/>
+      <c r="F33" s="31"/>
       <c r="G33" s="29"/>
       <c r="H33" s="25"/>
     </row>
@@ -1816,11 +1474,11 @@
         <v>24</v>
       </c>
       <c r="C34" s="25" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="D34" s="26"/>
       <c r="E34" s="27"/>
-      <c r="F34" s="28"/>
+      <c r="F34" s="31"/>
       <c r="G34" s="29"/>
       <c r="H34" s="25"/>
     </row>
@@ -1830,45 +1488,57 @@
         <v>25</v>
       </c>
       <c r="C35" s="25" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="D35" s="26"/>
       <c r="E35" s="27"/>
-      <c r="F35" s="28"/>
+      <c r="F35" s="31"/>
       <c r="G35" s="29"/>
       <c r="H35" s="25"/>
     </row>
-    <row r="36" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="12"/>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
-    </row>
-    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="12"/>
-      <c r="B37" s="12"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
-      <c r="H37" s="12"/>
-    </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="12"/>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="12"/>
-      <c r="E38" s="12"/>
-      <c r="F38" s="12"/>
-      <c r="G38" s="12"/>
-      <c r="H38" s="12"/>
-    </row>
-    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="23"/>
+      <c r="B36" s="24" t="n">
+        <v>26</v>
+      </c>
+      <c r="C36" s="25" t="s">
+        <v>56</v>
+      </c>
+      <c r="D36" s="26"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="25"/>
+    </row>
+    <row r="37" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="23"/>
+      <c r="B37" s="24" t="n">
+        <v>27</v>
+      </c>
+      <c r="C37" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="D37" s="26"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="29"/>
+      <c r="H37" s="25"/>
+    </row>
+    <row r="38" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="23"/>
+      <c r="B38" s="24" t="n">
+        <v>28</v>
+      </c>
+      <c r="C38" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="D38" s="26"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="29"/>
+      <c r="H38" s="25"/>
+    </row>
+    <row r="39" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="12"/>
       <c r="B39" s="12"/>
       <c r="C39" s="12"/>
@@ -1918,7 +1588,7 @@
       <c r="G43" s="12"/>
       <c r="H43" s="12"/>
     </row>
-    <row r="44" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="12"/>
       <c r="B44" s="12"/>
       <c r="C44" s="12"/>
@@ -1927,154 +1597,6 @@
       <c r="F44" s="12"/>
       <c r="G44" s="12"/>
       <c r="H44" s="12"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
-      <c r="L44" s="1"/>
-      <c r="M44" s="1"/>
-      <c r="N44" s="1"/>
-      <c r="O44" s="1"/>
-      <c r="P44" s="1"/>
-      <c r="Q44" s="1"/>
-      <c r="R44" s="1"/>
-      <c r="S44" s="1"/>
-      <c r="T44" s="1"/>
-      <c r="U44" s="1"/>
-      <c r="V44" s="1"/>
-      <c r="W44" s="1"/>
-      <c r="X44" s="1"/>
-      <c r="Y44" s="1"/>
-      <c r="Z44" s="1"/>
-      <c r="AA44" s="1"/>
-      <c r="AB44" s="1"/>
-      <c r="AC44" s="1"/>
-      <c r="AD44" s="1"/>
-      <c r="AE44" s="1"/>
-      <c r="AF44" s="1"/>
-      <c r="AG44" s="1"/>
-      <c r="AH44" s="1"/>
-      <c r="AI44" s="1"/>
-      <c r="AJ44" s="1"/>
-      <c r="AK44" s="1"/>
-      <c r="AL44" s="1"/>
-      <c r="AM44" s="1"/>
-      <c r="AN44" s="1"/>
-      <c r="AO44" s="1"/>
-      <c r="AP44" s="1"/>
-      <c r="AQ44" s="1"/>
-      <c r="AR44" s="1"/>
-      <c r="AS44" s="1"/>
-      <c r="AT44" s="1"/>
-      <c r="AU44" s="1"/>
-      <c r="AV44" s="1"/>
-      <c r="AW44" s="1"/>
-      <c r="AX44" s="1"/>
-      <c r="AY44" s="1"/>
-      <c r="AZ44" s="1"/>
-      <c r="BA44" s="1"/>
-      <c r="BB44" s="1"/>
-      <c r="BC44" s="1"/>
-      <c r="BD44" s="1"/>
-      <c r="BE44" s="1"/>
-      <c r="BF44" s="1"/>
-      <c r="BG44" s="1"/>
-      <c r="BH44" s="1"/>
-      <c r="BI44" s="1"/>
-      <c r="BJ44" s="1"/>
-      <c r="BK44" s="1"/>
-      <c r="BL44" s="1"/>
-      <c r="BM44" s="1"/>
-      <c r="BN44" s="1"/>
-      <c r="BO44" s="1"/>
-      <c r="BP44" s="1"/>
-      <c r="BQ44" s="1"/>
-      <c r="BR44" s="1"/>
-      <c r="BS44" s="1"/>
-      <c r="BT44" s="1"/>
-      <c r="BU44" s="1"/>
-      <c r="BV44" s="1"/>
-      <c r="BW44" s="1"/>
-      <c r="BX44" s="1"/>
-      <c r="BY44" s="1"/>
-      <c r="BZ44" s="1"/>
-      <c r="CA44" s="1"/>
-      <c r="CB44" s="1"/>
-      <c r="CC44" s="1"/>
-      <c r="CD44" s="1"/>
-      <c r="CE44" s="1"/>
-      <c r="CF44" s="1"/>
-      <c r="CG44" s="1"/>
-      <c r="CH44" s="1"/>
-      <c r="CI44" s="1"/>
-      <c r="CJ44" s="1"/>
-      <c r="CK44" s="1"/>
-      <c r="CL44" s="1"/>
-      <c r="CM44" s="1"/>
-      <c r="CN44" s="1"/>
-      <c r="CO44" s="1"/>
-      <c r="CP44" s="1"/>
-      <c r="CQ44" s="1"/>
-      <c r="CR44" s="1"/>
-      <c r="CS44" s="1"/>
-      <c r="CT44" s="1"/>
-      <c r="CU44" s="1"/>
-      <c r="CV44" s="1"/>
-      <c r="CW44" s="1"/>
-      <c r="CX44" s="1"/>
-      <c r="CY44" s="1"/>
-      <c r="CZ44" s="1"/>
-      <c r="DA44" s="1"/>
-      <c r="DB44" s="1"/>
-      <c r="DC44" s="1"/>
-      <c r="DD44" s="1"/>
-      <c r="DE44" s="1"/>
-      <c r="DF44" s="1"/>
-      <c r="DG44" s="1"/>
-      <c r="DH44" s="1"/>
-      <c r="DI44" s="1"/>
-      <c r="DJ44" s="1"/>
-      <c r="DK44" s="1"/>
-      <c r="DL44" s="1"/>
-      <c r="DM44" s="1"/>
-      <c r="DN44" s="1"/>
-      <c r="DO44" s="1"/>
-      <c r="DP44" s="1"/>
-      <c r="DQ44" s="1"/>
-      <c r="DR44" s="1"/>
-      <c r="DS44" s="1"/>
-      <c r="DT44" s="1"/>
-      <c r="DU44" s="1"/>
-      <c r="DV44" s="1"/>
-      <c r="DW44" s="1"/>
-      <c r="DX44" s="1"/>
-      <c r="DY44" s="1"/>
-      <c r="DZ44" s="1"/>
-      <c r="EA44" s="1"/>
-      <c r="EB44" s="1"/>
-      <c r="EC44" s="1"/>
-      <c r="ED44" s="1"/>
-      <c r="EE44" s="1"/>
-      <c r="EF44" s="1"/>
-      <c r="EG44" s="1"/>
-      <c r="EH44" s="1"/>
-      <c r="EI44" s="1"/>
-      <c r="EJ44" s="1"/>
-      <c r="EK44" s="1"/>
-      <c r="EL44" s="1"/>
-      <c r="EM44" s="1"/>
-      <c r="EN44" s="1"/>
-      <c r="EO44" s="1"/>
-      <c r="EP44" s="1"/>
-      <c r="EQ44" s="1"/>
-      <c r="ER44" s="1"/>
-      <c r="ES44" s="1"/>
-      <c r="ET44" s="1"/>
-      <c r="EU44" s="1"/>
-      <c r="EV44" s="1"/>
-      <c r="EW44" s="1"/>
-      <c r="EX44" s="1"/>
-      <c r="EY44" s="1"/>
-      <c r="EZ44" s="1"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="12"/>
@@ -2096,7 +1618,7 @@
       <c r="G46" s="12"/>
       <c r="H46" s="12"/>
     </row>
-    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="12"/>
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
@@ -2105,6 +1627,154 @@
       <c r="F47" s="12"/>
       <c r="G47" s="12"/>
       <c r="H47" s="12"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
+      <c r="M47" s="1"/>
+      <c r="N47" s="1"/>
+      <c r="O47" s="1"/>
+      <c r="P47" s="1"/>
+      <c r="Q47" s="1"/>
+      <c r="R47" s="1"/>
+      <c r="S47" s="1"/>
+      <c r="T47" s="1"/>
+      <c r="U47" s="1"/>
+      <c r="V47" s="1"/>
+      <c r="W47" s="1"/>
+      <c r="X47" s="1"/>
+      <c r="Y47" s="1"/>
+      <c r="Z47" s="1"/>
+      <c r="AA47" s="1"/>
+      <c r="AB47" s="1"/>
+      <c r="AC47" s="1"/>
+      <c r="AD47" s="1"/>
+      <c r="AE47" s="1"/>
+      <c r="AF47" s="1"/>
+      <c r="AG47" s="1"/>
+      <c r="AH47" s="1"/>
+      <c r="AI47" s="1"/>
+      <c r="AJ47" s="1"/>
+      <c r="AK47" s="1"/>
+      <c r="AL47" s="1"/>
+      <c r="AM47" s="1"/>
+      <c r="AN47" s="1"/>
+      <c r="AO47" s="1"/>
+      <c r="AP47" s="1"/>
+      <c r="AQ47" s="1"/>
+      <c r="AR47" s="1"/>
+      <c r="AS47" s="1"/>
+      <c r="AT47" s="1"/>
+      <c r="AU47" s="1"/>
+      <c r="AV47" s="1"/>
+      <c r="AW47" s="1"/>
+      <c r="AX47" s="1"/>
+      <c r="AY47" s="1"/>
+      <c r="AZ47" s="1"/>
+      <c r="BA47" s="1"/>
+      <c r="BB47" s="1"/>
+      <c r="BC47" s="1"/>
+      <c r="BD47" s="1"/>
+      <c r="BE47" s="1"/>
+      <c r="BF47" s="1"/>
+      <c r="BG47" s="1"/>
+      <c r="BH47" s="1"/>
+      <c r="BI47" s="1"/>
+      <c r="BJ47" s="1"/>
+      <c r="BK47" s="1"/>
+      <c r="BL47" s="1"/>
+      <c r="BM47" s="1"/>
+      <c r="BN47" s="1"/>
+      <c r="BO47" s="1"/>
+      <c r="BP47" s="1"/>
+      <c r="BQ47" s="1"/>
+      <c r="BR47" s="1"/>
+      <c r="BS47" s="1"/>
+      <c r="BT47" s="1"/>
+      <c r="BU47" s="1"/>
+      <c r="BV47" s="1"/>
+      <c r="BW47" s="1"/>
+      <c r="BX47" s="1"/>
+      <c r="BY47" s="1"/>
+      <c r="BZ47" s="1"/>
+      <c r="CA47" s="1"/>
+      <c r="CB47" s="1"/>
+      <c r="CC47" s="1"/>
+      <c r="CD47" s="1"/>
+      <c r="CE47" s="1"/>
+      <c r="CF47" s="1"/>
+      <c r="CG47" s="1"/>
+      <c r="CH47" s="1"/>
+      <c r="CI47" s="1"/>
+      <c r="CJ47" s="1"/>
+      <c r="CK47" s="1"/>
+      <c r="CL47" s="1"/>
+      <c r="CM47" s="1"/>
+      <c r="CN47" s="1"/>
+      <c r="CO47" s="1"/>
+      <c r="CP47" s="1"/>
+      <c r="CQ47" s="1"/>
+      <c r="CR47" s="1"/>
+      <c r="CS47" s="1"/>
+      <c r="CT47" s="1"/>
+      <c r="CU47" s="1"/>
+      <c r="CV47" s="1"/>
+      <c r="CW47" s="1"/>
+      <c r="CX47" s="1"/>
+      <c r="CY47" s="1"/>
+      <c r="CZ47" s="1"/>
+      <c r="DA47" s="1"/>
+      <c r="DB47" s="1"/>
+      <c r="DC47" s="1"/>
+      <c r="DD47" s="1"/>
+      <c r="DE47" s="1"/>
+      <c r="DF47" s="1"/>
+      <c r="DG47" s="1"/>
+      <c r="DH47" s="1"/>
+      <c r="DI47" s="1"/>
+      <c r="DJ47" s="1"/>
+      <c r="DK47" s="1"/>
+      <c r="DL47" s="1"/>
+      <c r="DM47" s="1"/>
+      <c r="DN47" s="1"/>
+      <c r="DO47" s="1"/>
+      <c r="DP47" s="1"/>
+      <c r="DQ47" s="1"/>
+      <c r="DR47" s="1"/>
+      <c r="DS47" s="1"/>
+      <c r="DT47" s="1"/>
+      <c r="DU47" s="1"/>
+      <c r="DV47" s="1"/>
+      <c r="DW47" s="1"/>
+      <c r="DX47" s="1"/>
+      <c r="DY47" s="1"/>
+      <c r="DZ47" s="1"/>
+      <c r="EA47" s="1"/>
+      <c r="EB47" s="1"/>
+      <c r="EC47" s="1"/>
+      <c r="ED47" s="1"/>
+      <c r="EE47" s="1"/>
+      <c r="EF47" s="1"/>
+      <c r="EG47" s="1"/>
+      <c r="EH47" s="1"/>
+      <c r="EI47" s="1"/>
+      <c r="EJ47" s="1"/>
+      <c r="EK47" s="1"/>
+      <c r="EL47" s="1"/>
+      <c r="EM47" s="1"/>
+      <c r="EN47" s="1"/>
+      <c r="EO47" s="1"/>
+      <c r="EP47" s="1"/>
+      <c r="EQ47" s="1"/>
+      <c r="ER47" s="1"/>
+      <c r="ES47" s="1"/>
+      <c r="ET47" s="1"/>
+      <c r="EU47" s="1"/>
+      <c r="EV47" s="1"/>
+      <c r="EW47" s="1"/>
+      <c r="EX47" s="1"/>
+      <c r="EY47" s="1"/>
+      <c r="EZ47" s="1"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="12"/>
@@ -2234,7 +1904,7 @@
       <c r="E60" s="12"/>
       <c r="F60" s="12"/>
       <c r="G60" s="12"/>
-      <c r="EZ60" s="8"/>
+      <c r="H60" s="12"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="12"/>
@@ -2244,7 +1914,7 @@
       <c r="E61" s="12"/>
       <c r="F61" s="12"/>
       <c r="G61" s="12"/>
-      <c r="EZ61" s="8"/>
+      <c r="H61" s="12"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="12"/>
@@ -2254,7 +1924,7 @@
       <c r="E62" s="12"/>
       <c r="F62" s="12"/>
       <c r="G62" s="12"/>
-      <c r="EZ62" s="8"/>
+      <c r="H62" s="12"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="12"/>
@@ -2274,7 +1944,7 @@
       <c r="E64" s="12"/>
       <c r="F64" s="12"/>
       <c r="G64" s="12"/>
-      <c r="H64" s="12"/>
+      <c r="EZ64" s="8"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="12"/>
@@ -2284,7 +1954,7 @@
       <c r="E65" s="12"/>
       <c r="F65" s="12"/>
       <c r="G65" s="12"/>
-      <c r="H65" s="12"/>
+      <c r="EZ65" s="8"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="12"/>
@@ -2294,7 +1964,7 @@
       <c r="E66" s="12"/>
       <c r="F66" s="12"/>
       <c r="G66" s="12"/>
-      <c r="H66" s="12"/>
+      <c r="EZ66" s="8"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="12"/>
@@ -10768,6 +10438,36 @@
     </row>
     <row r="914" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A914" s="12"/>
+      <c r="B914" s="12"/>
+      <c r="C914" s="12"/>
+      <c r="D914" s="12"/>
+      <c r="E914" s="12"/>
+      <c r="F914" s="12"/>
+      <c r="G914" s="12"/>
+      <c r="H914" s="12"/>
+    </row>
+    <row r="915" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A915" s="12"/>
+      <c r="B915" s="12"/>
+      <c r="C915" s="12"/>
+      <c r="D915" s="12"/>
+      <c r="E915" s="12"/>
+      <c r="F915" s="12"/>
+      <c r="G915" s="12"/>
+      <c r="H915" s="12"/>
+    </row>
+    <row r="916" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A916" s="12"/>
+      <c r="B916" s="12"/>
+      <c r="C916" s="12"/>
+      <c r="D916" s="12"/>
+      <c r="E916" s="12"/>
+      <c r="F916" s="12"/>
+      <c r="G916" s="12"/>
+      <c r="H916" s="12"/>
+    </row>
+    <row r="917" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A917" s="12"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
@@ -10794,15 +10494,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="31" width="3.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="31" width="88.33"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="3" style="31" width="10.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="3.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="33" width="88.33"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="3" style="33" width="10.78"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="105" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="32" t="s">
-        <v>47</v>
+      <c r="B2" s="34" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
3 further unit tests
</commit_message>
<xml_diff>
--- a/docs/TestPlan.xlsx
+++ b/docs/TestPlan.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
   <si>
     <t xml:space="preserve">TEST CASE PLANNING AND EXECUTION</t>
   </si>
@@ -146,25 +146,7 @@
     <t xml:space="preserve">Test Pass – The submit button can be selected and the data is imported</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Test Expected Fail (Due to pytest timeout) -</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Century Gothic"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> The submit button can be selected and the data is imported</t>
-    </r>
+    <t xml:space="preserve">Test Expected Fail (Due to pytest timeout) - The submit button can be selected and the data is imported</t>
   </si>
   <si>
     <t xml:space="preserve">Test times out after 3 seconds, set as XFAIL when it times out passes as it shows data is being imported</t>
@@ -221,6 +203,15 @@
     <t xml:space="preserve">All values can be edited and stay the selected values when the submit button is selected – DB 1 (Clickhouse)</t>
   </si>
   <si>
+    <t xml:space="preserve">Test Pass – The submit button can be selected and all the changed fields remain changed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Expected Fail (Due to pytest timeout) - The submit button can be selected but times out due to data import</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XFAIL</t>
+  </si>
+  <si>
     <t xml:space="preserve">All values can be edited and stay the selected values when the submit button is selected – DB 2 (PostgreSQL)</t>
   </si>
   <si>
@@ -238,7 +229,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -325,18 +316,6 @@
       <name val="Century Gothic"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Century Gothic"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Century Gothic"/>
-      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -532,7 +511,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -645,7 +624,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -653,23 +632,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="12" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="1" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="6" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="6" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="2" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -755,9 +722,9 @@
   <dimension ref="A1:EZ917"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H27" activeCellId="0" sqref="H27"/>
+      <selection pane="bottomLeft" activeCell="H36" activeCellId="0" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1149,7 +1116,7 @@
       <c r="D14" s="26" t="n">
         <v>45375</v>
       </c>
-      <c r="E14" s="30" t="s">
+      <c r="E14" s="27" t="s">
         <v>27</v>
       </c>
       <c r="F14" s="28" t="s">
@@ -1171,7 +1138,7 @@
       <c r="D15" s="26" t="n">
         <v>45375</v>
       </c>
-      <c r="E15" s="30" t="s">
+      <c r="E15" s="27" t="s">
         <v>29</v>
       </c>
       <c r="F15" s="28" t="s">
@@ -1193,7 +1160,7 @@
       <c r="D16" s="26" t="n">
         <v>45375</v>
       </c>
-      <c r="E16" s="30" t="s">
+      <c r="E16" s="27" t="s">
         <v>31</v>
       </c>
       <c r="F16" s="28" t="s">
@@ -1215,7 +1182,7 @@
       <c r="D17" s="26" t="n">
         <v>45375</v>
       </c>
-      <c r="E17" s="30" t="s">
+      <c r="E17" s="27" t="s">
         <v>33</v>
       </c>
       <c r="F17" s="28" t="s">
@@ -1237,7 +1204,7 @@
       <c r="D18" s="26" t="n">
         <v>45375</v>
       </c>
-      <c r="E18" s="30" t="s">
+      <c r="E18" s="27" t="s">
         <v>35</v>
       </c>
       <c r="F18" s="28" t="s">
@@ -1259,10 +1226,10 @@
       <c r="D19" s="26" t="n">
         <v>45375</v>
       </c>
-      <c r="E19" s="30" t="s">
+      <c r="E19" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="F19" s="31" t="s">
+      <c r="F19" s="28" t="s">
         <v>38</v>
       </c>
       <c r="G19" s="29" t="s">
@@ -1282,7 +1249,7 @@
       </c>
       <c r="D20" s="26"/>
       <c r="E20" s="27"/>
-      <c r="F20" s="31"/>
+      <c r="F20" s="28"/>
       <c r="G20" s="29"/>
       <c r="H20" s="25"/>
     </row>
@@ -1296,7 +1263,7 @@
       </c>
       <c r="D21" s="26"/>
       <c r="E21" s="27"/>
-      <c r="F21" s="31"/>
+      <c r="F21" s="28"/>
       <c r="G21" s="29"/>
       <c r="H21" s="25"/>
     </row>
@@ -1310,7 +1277,7 @@
       </c>
       <c r="D22" s="26"/>
       <c r="E22" s="27"/>
-      <c r="F22" s="31"/>
+      <c r="F22" s="28"/>
       <c r="G22" s="29"/>
       <c r="H22" s="25"/>
     </row>
@@ -1324,7 +1291,7 @@
       </c>
       <c r="D23" s="26"/>
       <c r="E23" s="27"/>
-      <c r="F23" s="31"/>
+      <c r="F23" s="28"/>
       <c r="G23" s="29"/>
       <c r="H23" s="25"/>
     </row>
@@ -1338,7 +1305,7 @@
       </c>
       <c r="D24" s="26"/>
       <c r="E24" s="27"/>
-      <c r="F24" s="31"/>
+      <c r="F24" s="28"/>
       <c r="G24" s="29"/>
       <c r="H24" s="25"/>
     </row>
@@ -1352,7 +1319,7 @@
       </c>
       <c r="D25" s="26"/>
       <c r="E25" s="27"/>
-      <c r="F25" s="31"/>
+      <c r="F25" s="28"/>
       <c r="G25" s="29"/>
       <c r="H25" s="25"/>
     </row>
@@ -1366,7 +1333,7 @@
       </c>
       <c r="D26" s="26"/>
       <c r="E26" s="27"/>
-      <c r="F26" s="31"/>
+      <c r="F26" s="28"/>
       <c r="G26" s="29"/>
       <c r="H26" s="25"/>
     </row>
@@ -1380,7 +1347,7 @@
       </c>
       <c r="D27" s="26"/>
       <c r="E27" s="27"/>
-      <c r="F27" s="31"/>
+      <c r="F27" s="28"/>
       <c r="G27" s="29"/>
       <c r="H27" s="25"/>
     </row>
@@ -1394,7 +1361,7 @@
       </c>
       <c r="D28" s="26"/>
       <c r="E28" s="27"/>
-      <c r="F28" s="31"/>
+      <c r="F28" s="28"/>
       <c r="G28" s="29"/>
       <c r="H28" s="25"/>
     </row>
@@ -1408,7 +1375,7 @@
       </c>
       <c r="D29" s="26"/>
       <c r="E29" s="27"/>
-      <c r="F29" s="31"/>
+      <c r="F29" s="28"/>
       <c r="G29" s="29"/>
       <c r="H29" s="25"/>
     </row>
@@ -1422,7 +1389,7 @@
       </c>
       <c r="D30" s="26"/>
       <c r="E30" s="27"/>
-      <c r="F30" s="31"/>
+      <c r="F30" s="28"/>
       <c r="G30" s="29"/>
       <c r="H30" s="25"/>
     </row>
@@ -1436,7 +1403,7 @@
       </c>
       <c r="D31" s="26"/>
       <c r="E31" s="27"/>
-      <c r="F31" s="31"/>
+      <c r="F31" s="28"/>
       <c r="G31" s="29"/>
       <c r="H31" s="25"/>
     </row>
@@ -1450,7 +1417,7 @@
       </c>
       <c r="D32" s="26"/>
       <c r="E32" s="27"/>
-      <c r="F32" s="31"/>
+      <c r="F32" s="28"/>
       <c r="G32" s="29"/>
       <c r="H32" s="25"/>
     </row>
@@ -1464,7 +1431,7 @@
       </c>
       <c r="D33" s="26"/>
       <c r="E33" s="27"/>
-      <c r="F33" s="31"/>
+      <c r="F33" s="28"/>
       <c r="G33" s="29"/>
       <c r="H33" s="25"/>
     </row>
@@ -1478,7 +1445,7 @@
       </c>
       <c r="D34" s="26"/>
       <c r="E34" s="27"/>
-      <c r="F34" s="31"/>
+      <c r="F34" s="28"/>
       <c r="G34" s="29"/>
       <c r="H34" s="25"/>
     </row>
@@ -1492,7 +1459,7 @@
       </c>
       <c r="D35" s="26"/>
       <c r="E35" s="27"/>
-      <c r="F35" s="31"/>
+      <c r="F35" s="28"/>
       <c r="G35" s="29"/>
       <c r="H35" s="25"/>
     </row>
@@ -1504,23 +1471,33 @@
       <c r="C36" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="D36" s="26"/>
-      <c r="E36" s="27"/>
-      <c r="F36" s="31"/>
-      <c r="G36" s="29"/>
-      <c r="H36" s="25"/>
+      <c r="D36" s="26" t="n">
+        <v>45375</v>
+      </c>
+      <c r="E36" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="F36" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="G36" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="H36" s="25" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="23"/>
       <c r="B37" s="24" t="n">
         <v>27</v>
       </c>
-      <c r="C37" s="32" t="s">
-        <v>57</v>
+      <c r="C37" s="25" t="s">
+        <v>60</v>
       </c>
       <c r="D37" s="26"/>
       <c r="E37" s="27"/>
-      <c r="F37" s="31"/>
+      <c r="F37" s="28"/>
       <c r="G37" s="29"/>
       <c r="H37" s="25"/>
     </row>
@@ -1529,12 +1506,12 @@
       <c r="B38" s="24" t="n">
         <v>28</v>
       </c>
-      <c r="C38" s="32" t="s">
-        <v>58</v>
+      <c r="C38" s="25" t="s">
+        <v>61</v>
       </c>
       <c r="D38" s="26"/>
       <c r="E38" s="27"/>
-      <c r="F38" s="31"/>
+      <c r="F38" s="28"/>
       <c r="G38" s="29"/>
       <c r="H38" s="25"/>
     </row>
@@ -10494,15 +10471,15 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="33" width="3.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="33" width="88.33"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="3" style="33" width="10.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="30" width="3.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="30" width="88.33"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="3" style="30" width="10.78"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="105" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B2" s="34" t="s">
-        <v>59</v>
+      <c r="B2" s="31" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Clickhouse write benchmark + minor updates
</commit_message>
<xml_diff>
--- a/docs/TestPlan.xlsx
+++ b/docs/TestPlan.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="72">
   <si>
     <t xml:space="preserve">TEST CASE PLANNING AND EXECUTION</t>
   </si>
@@ -200,6 +200,226 @@
     <t xml:space="preserve">Submit Button can be selected and data ingressed for each Database type – DB 3 (TimescaleDB)</t>
   </si>
   <si>
+    <t xml:space="preserve">Downsampling Toggle can be selected for DB 4 – (ArcticDB)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Increment the Downsample Number Input for each Database type – DB 4 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">ArcticDB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Set the Downsample Number Input for each Database type – DB 4 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">ArcticDB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Change the start date of each Database type – DB 4 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">ArcticDB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Change the end date of each Database type – DB 4 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">ArcticDB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Change the start time of each Database type – DB 4 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">ArcticDB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Change the end time of each Database type – DB 4 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">ArcticDB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Submit Button can be selected and data ingressed for each Database type – DB 4 (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">ArcticDB</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Century Gothic"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">)</t>
+    </r>
+  </si>
+  <si>
     <t xml:space="preserve">All values can be edited and stay the selected values when the submit button is selected – DB 1 (Clickhouse)</t>
   </si>
   <si>
@@ -215,7 +435,10 @@
     <t xml:space="preserve">All values can be edited and stay the selected values when the submit button is selected – DB 2 (PostgreSQL)</t>
   </si>
   <si>
-    <t xml:space="preserve">All values can be edited and stay the selected values when the submit button is selected – DB 1 (TimescaleDB)</t>
+    <t xml:space="preserve">All values can be edited and stay the selected values when the submit button is selected – DB 3 (TimescaleDB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All values can be edited and stay the selected values when the submit button is selected – DB 4 (ArcticDB)</t>
   </si>
   <si>
     <t xml:space="preserve">Any articles, templates, or information provided by Smartsheet on the website are for reference only. While we strive to keep the information up to date and correct, we make no representations or warranties of any kind, express or implied, about the completeness, accuracy, reliability, suitability, or availability with respect to the website or the information, articles, templates, or related graphics contained on the website. Any reliance you place on such information is therefore strictly at your own risk. </t>
@@ -229,7 +452,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -316,6 +539,12 @@
       <name val="Century Gothic"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Century Gothic"/>
+      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -636,7 +865,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="6" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="6" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="2" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -719,12 +948,12 @@
     <tabColor rgb="FF8497B0"/>
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:EZ917"/>
+  <dimension ref="A1:EZ926"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H36" activeCellId="0" sqref="H36"/>
+      <selection pane="bottomLeft" activeCell="C47" activeCellId="0" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1471,21 +1700,11 @@
       <c r="C36" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="D36" s="26" t="n">
-        <v>45375</v>
-      </c>
-      <c r="E36" s="27" t="s">
-        <v>57</v>
-      </c>
-      <c r="F36" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="G36" s="29" t="s">
-        <v>59</v>
-      </c>
-      <c r="H36" s="25" t="s">
-        <v>39</v>
-      </c>
+      <c r="D36" s="26"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="29"/>
+      <c r="H36" s="25"/>
     </row>
     <row r="37" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="23"/>
@@ -1493,7 +1712,7 @@
         <v>27</v>
       </c>
       <c r="C37" s="25" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D37" s="26"/>
       <c r="E37" s="27"/>
@@ -1507,7 +1726,7 @@
         <v>28</v>
       </c>
       <c r="C38" s="25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D38" s="26"/>
       <c r="E38" s="27"/>
@@ -1515,245 +1734,143 @@
       <c r="G38" s="29"/>
       <c r="H38" s="25"/>
     </row>
-    <row r="39" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="12"/>
-      <c r="B39" s="12"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12"/>
-      <c r="F39" s="12"/>
-      <c r="G39" s="12"/>
-      <c r="H39" s="12"/>
-    </row>
-    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="12"/>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="12"/>
-      <c r="G40" s="12"/>
-      <c r="H40" s="12"/>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="12"/>
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="12"/>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="12"/>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
-      <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="12"/>
-      <c r="G42" s="12"/>
-      <c r="H42" s="12"/>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="12"/>
-      <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="12"/>
-      <c r="G43" s="12"/>
-      <c r="H43" s="12"/>
-    </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="12"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="12"/>
-      <c r="D44" s="12"/>
-      <c r="E44" s="12"/>
-      <c r="F44" s="12"/>
-      <c r="G44" s="12"/>
-      <c r="H44" s="12"/>
-    </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="12"/>
-      <c r="B45" s="12"/>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="12"/>
-      <c r="B46" s="12"/>
-      <c r="C46" s="12"/>
-      <c r="D46" s="12"/>
-      <c r="E46" s="12"/>
-      <c r="F46" s="12"/>
-      <c r="G46" s="12"/>
-      <c r="H46" s="12"/>
-    </row>
-    <row r="47" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="12"/>
-      <c r="B47" s="12"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="12"/>
-      <c r="E47" s="12"/>
-      <c r="F47" s="12"/>
-      <c r="G47" s="12"/>
-      <c r="H47" s="12"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="1"/>
-      <c r="L47" s="1"/>
-      <c r="M47" s="1"/>
-      <c r="N47" s="1"/>
-      <c r="O47" s="1"/>
-      <c r="P47" s="1"/>
-      <c r="Q47" s="1"/>
-      <c r="R47" s="1"/>
-      <c r="S47" s="1"/>
-      <c r="T47" s="1"/>
-      <c r="U47" s="1"/>
-      <c r="V47" s="1"/>
-      <c r="W47" s="1"/>
-      <c r="X47" s="1"/>
-      <c r="Y47" s="1"/>
-      <c r="Z47" s="1"/>
-      <c r="AA47" s="1"/>
-      <c r="AB47" s="1"/>
-      <c r="AC47" s="1"/>
-      <c r="AD47" s="1"/>
-      <c r="AE47" s="1"/>
-      <c r="AF47" s="1"/>
-      <c r="AG47" s="1"/>
-      <c r="AH47" s="1"/>
-      <c r="AI47" s="1"/>
-      <c r="AJ47" s="1"/>
-      <c r="AK47" s="1"/>
-      <c r="AL47" s="1"/>
-      <c r="AM47" s="1"/>
-      <c r="AN47" s="1"/>
-      <c r="AO47" s="1"/>
-      <c r="AP47" s="1"/>
-      <c r="AQ47" s="1"/>
-      <c r="AR47" s="1"/>
-      <c r="AS47" s="1"/>
-      <c r="AT47" s="1"/>
-      <c r="AU47" s="1"/>
-      <c r="AV47" s="1"/>
-      <c r="AW47" s="1"/>
-      <c r="AX47" s="1"/>
-      <c r="AY47" s="1"/>
-      <c r="AZ47" s="1"/>
-      <c r="BA47" s="1"/>
-      <c r="BB47" s="1"/>
-      <c r="BC47" s="1"/>
-      <c r="BD47" s="1"/>
-      <c r="BE47" s="1"/>
-      <c r="BF47" s="1"/>
-      <c r="BG47" s="1"/>
-      <c r="BH47" s="1"/>
-      <c r="BI47" s="1"/>
-      <c r="BJ47" s="1"/>
-      <c r="BK47" s="1"/>
-      <c r="BL47" s="1"/>
-      <c r="BM47" s="1"/>
-      <c r="BN47" s="1"/>
-      <c r="BO47" s="1"/>
-      <c r="BP47" s="1"/>
-      <c r="BQ47" s="1"/>
-      <c r="BR47" s="1"/>
-      <c r="BS47" s="1"/>
-      <c r="BT47" s="1"/>
-      <c r="BU47" s="1"/>
-      <c r="BV47" s="1"/>
-      <c r="BW47" s="1"/>
-      <c r="BX47" s="1"/>
-      <c r="BY47" s="1"/>
-      <c r="BZ47" s="1"/>
-      <c r="CA47" s="1"/>
-      <c r="CB47" s="1"/>
-      <c r="CC47" s="1"/>
-      <c r="CD47" s="1"/>
-      <c r="CE47" s="1"/>
-      <c r="CF47" s="1"/>
-      <c r="CG47" s="1"/>
-      <c r="CH47" s="1"/>
-      <c r="CI47" s="1"/>
-      <c r="CJ47" s="1"/>
-      <c r="CK47" s="1"/>
-      <c r="CL47" s="1"/>
-      <c r="CM47" s="1"/>
-      <c r="CN47" s="1"/>
-      <c r="CO47" s="1"/>
-      <c r="CP47" s="1"/>
-      <c r="CQ47" s="1"/>
-      <c r="CR47" s="1"/>
-      <c r="CS47" s="1"/>
-      <c r="CT47" s="1"/>
-      <c r="CU47" s="1"/>
-      <c r="CV47" s="1"/>
-      <c r="CW47" s="1"/>
-      <c r="CX47" s="1"/>
-      <c r="CY47" s="1"/>
-      <c r="CZ47" s="1"/>
-      <c r="DA47" s="1"/>
-      <c r="DB47" s="1"/>
-      <c r="DC47" s="1"/>
-      <c r="DD47" s="1"/>
-      <c r="DE47" s="1"/>
-      <c r="DF47" s="1"/>
-      <c r="DG47" s="1"/>
-      <c r="DH47" s="1"/>
-      <c r="DI47" s="1"/>
-      <c r="DJ47" s="1"/>
-      <c r="DK47" s="1"/>
-      <c r="DL47" s="1"/>
-      <c r="DM47" s="1"/>
-      <c r="DN47" s="1"/>
-      <c r="DO47" s="1"/>
-      <c r="DP47" s="1"/>
-      <c r="DQ47" s="1"/>
-      <c r="DR47" s="1"/>
-      <c r="DS47" s="1"/>
-      <c r="DT47" s="1"/>
-      <c r="DU47" s="1"/>
-      <c r="DV47" s="1"/>
-      <c r="DW47" s="1"/>
-      <c r="DX47" s="1"/>
-      <c r="DY47" s="1"/>
-      <c r="DZ47" s="1"/>
-      <c r="EA47" s="1"/>
-      <c r="EB47" s="1"/>
-      <c r="EC47" s="1"/>
-      <c r="ED47" s="1"/>
-      <c r="EE47" s="1"/>
-      <c r="EF47" s="1"/>
-      <c r="EG47" s="1"/>
-      <c r="EH47" s="1"/>
-      <c r="EI47" s="1"/>
-      <c r="EJ47" s="1"/>
-      <c r="EK47" s="1"/>
-      <c r="EL47" s="1"/>
-      <c r="EM47" s="1"/>
-      <c r="EN47" s="1"/>
-      <c r="EO47" s="1"/>
-      <c r="EP47" s="1"/>
-      <c r="EQ47" s="1"/>
-      <c r="ER47" s="1"/>
-      <c r="ES47" s="1"/>
-      <c r="ET47" s="1"/>
-      <c r="EU47" s="1"/>
-      <c r="EV47" s="1"/>
-      <c r="EW47" s="1"/>
-      <c r="EX47" s="1"/>
-      <c r="EY47" s="1"/>
-      <c r="EZ47" s="1"/>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="23"/>
+      <c r="B39" s="24" t="n">
+        <v>29</v>
+      </c>
+      <c r="C39" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="D39" s="26"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="28"/>
+      <c r="G39" s="29"/>
+      <c r="H39" s="25"/>
+    </row>
+    <row r="40" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="23"/>
+      <c r="B40" s="24" t="n">
+        <v>30</v>
+      </c>
+      <c r="C40" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="D40" s="26"/>
+      <c r="E40" s="27"/>
+      <c r="F40" s="28"/>
+      <c r="G40" s="29"/>
+      <c r="H40" s="25"/>
+    </row>
+    <row r="41" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="23"/>
+      <c r="B41" s="24" t="n">
+        <v>31</v>
+      </c>
+      <c r="C41" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="D41" s="26"/>
+      <c r="E41" s="27"/>
+      <c r="F41" s="28"/>
+      <c r="G41" s="29"/>
+      <c r="H41" s="25"/>
+    </row>
+    <row r="42" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="23"/>
+      <c r="B42" s="24" t="n">
+        <v>32</v>
+      </c>
+      <c r="C42" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="D42" s="26"/>
+      <c r="E42" s="27"/>
+      <c r="F42" s="28"/>
+      <c r="G42" s="29"/>
+      <c r="H42" s="25"/>
+    </row>
+    <row r="43" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="23"/>
+      <c r="B43" s="24" t="n">
+        <v>33</v>
+      </c>
+      <c r="C43" s="25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D43" s="26"/>
+      <c r="E43" s="27"/>
+      <c r="F43" s="28"/>
+      <c r="G43" s="29"/>
+      <c r="H43" s="25"/>
+    </row>
+    <row r="44" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="23"/>
+      <c r="B44" s="24" t="n">
+        <v>34</v>
+      </c>
+      <c r="C44" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="D44" s="26" t="n">
+        <v>45375</v>
+      </c>
+      <c r="E44" s="27" t="s">
+        <v>65</v>
+      </c>
+      <c r="F44" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="G44" s="29" t="s">
+        <v>67</v>
+      </c>
+      <c r="H44" s="25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="23"/>
+      <c r="B45" s="24" t="n">
+        <v>35</v>
+      </c>
+      <c r="C45" s="25" t="s">
+        <v>68</v>
+      </c>
+      <c r="D45" s="26"/>
+      <c r="E45" s="27"/>
+      <c r="F45" s="28"/>
+      <c r="G45" s="29"/>
+      <c r="H45" s="25"/>
+    </row>
+    <row r="46" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="23"/>
+      <c r="B46" s="24" t="n">
+        <v>36</v>
+      </c>
+      <c r="C46" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="D46" s="26"/>
+      <c r="E46" s="27"/>
+      <c r="F46" s="28"/>
+      <c r="G46" s="29"/>
+      <c r="H46" s="25"/>
+    </row>
+    <row r="47" customFormat="false" ht="51.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="23"/>
+      <c r="B47" s="24" t="n">
+        <v>37</v>
+      </c>
+      <c r="C47" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="D47" s="26"/>
+      <c r="E47" s="27"/>
+      <c r="F47" s="28"/>
+      <c r="G47" s="29"/>
+      <c r="H47" s="25"/>
+    </row>
+    <row r="48" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="12"/>
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
@@ -1833,7 +1950,7 @@
       <c r="G55" s="12"/>
       <c r="H55" s="12"/>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" s="8" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="12"/>
       <c r="B56" s="12"/>
       <c r="C56" s="12"/>
@@ -1842,6 +1959,154 @@
       <c r="F56" s="12"/>
       <c r="G56" s="12"/>
       <c r="H56" s="12"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+      <c r="L56" s="1"/>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
+      <c r="O56" s="1"/>
+      <c r="P56" s="1"/>
+      <c r="Q56" s="1"/>
+      <c r="R56" s="1"/>
+      <c r="S56" s="1"/>
+      <c r="T56" s="1"/>
+      <c r="U56" s="1"/>
+      <c r="V56" s="1"/>
+      <c r="W56" s="1"/>
+      <c r="X56" s="1"/>
+      <c r="Y56" s="1"/>
+      <c r="Z56" s="1"/>
+      <c r="AA56" s="1"/>
+      <c r="AB56" s="1"/>
+      <c r="AC56" s="1"/>
+      <c r="AD56" s="1"/>
+      <c r="AE56" s="1"/>
+      <c r="AF56" s="1"/>
+      <c r="AG56" s="1"/>
+      <c r="AH56" s="1"/>
+      <c r="AI56" s="1"/>
+      <c r="AJ56" s="1"/>
+      <c r="AK56" s="1"/>
+      <c r="AL56" s="1"/>
+      <c r="AM56" s="1"/>
+      <c r="AN56" s="1"/>
+      <c r="AO56" s="1"/>
+      <c r="AP56" s="1"/>
+      <c r="AQ56" s="1"/>
+      <c r="AR56" s="1"/>
+      <c r="AS56" s="1"/>
+      <c r="AT56" s="1"/>
+      <c r="AU56" s="1"/>
+      <c r="AV56" s="1"/>
+      <c r="AW56" s="1"/>
+      <c r="AX56" s="1"/>
+      <c r="AY56" s="1"/>
+      <c r="AZ56" s="1"/>
+      <c r="BA56" s="1"/>
+      <c r="BB56" s="1"/>
+      <c r="BC56" s="1"/>
+      <c r="BD56" s="1"/>
+      <c r="BE56" s="1"/>
+      <c r="BF56" s="1"/>
+      <c r="BG56" s="1"/>
+      <c r="BH56" s="1"/>
+      <c r="BI56" s="1"/>
+      <c r="BJ56" s="1"/>
+      <c r="BK56" s="1"/>
+      <c r="BL56" s="1"/>
+      <c r="BM56" s="1"/>
+      <c r="BN56" s="1"/>
+      <c r="BO56" s="1"/>
+      <c r="BP56" s="1"/>
+      <c r="BQ56" s="1"/>
+      <c r="BR56" s="1"/>
+      <c r="BS56" s="1"/>
+      <c r="BT56" s="1"/>
+      <c r="BU56" s="1"/>
+      <c r="BV56" s="1"/>
+      <c r="BW56" s="1"/>
+      <c r="BX56" s="1"/>
+      <c r="BY56" s="1"/>
+      <c r="BZ56" s="1"/>
+      <c r="CA56" s="1"/>
+      <c r="CB56" s="1"/>
+      <c r="CC56" s="1"/>
+      <c r="CD56" s="1"/>
+      <c r="CE56" s="1"/>
+      <c r="CF56" s="1"/>
+      <c r="CG56" s="1"/>
+      <c r="CH56" s="1"/>
+      <c r="CI56" s="1"/>
+      <c r="CJ56" s="1"/>
+      <c r="CK56" s="1"/>
+      <c r="CL56" s="1"/>
+      <c r="CM56" s="1"/>
+      <c r="CN56" s="1"/>
+      <c r="CO56" s="1"/>
+      <c r="CP56" s="1"/>
+      <c r="CQ56" s="1"/>
+      <c r="CR56" s="1"/>
+      <c r="CS56" s="1"/>
+      <c r="CT56" s="1"/>
+      <c r="CU56" s="1"/>
+      <c r="CV56" s="1"/>
+      <c r="CW56" s="1"/>
+      <c r="CX56" s="1"/>
+      <c r="CY56" s="1"/>
+      <c r="CZ56" s="1"/>
+      <c r="DA56" s="1"/>
+      <c r="DB56" s="1"/>
+      <c r="DC56" s="1"/>
+      <c r="DD56" s="1"/>
+      <c r="DE56" s="1"/>
+      <c r="DF56" s="1"/>
+      <c r="DG56" s="1"/>
+      <c r="DH56" s="1"/>
+      <c r="DI56" s="1"/>
+      <c r="DJ56" s="1"/>
+      <c r="DK56" s="1"/>
+      <c r="DL56" s="1"/>
+      <c r="DM56" s="1"/>
+      <c r="DN56" s="1"/>
+      <c r="DO56" s="1"/>
+      <c r="DP56" s="1"/>
+      <c r="DQ56" s="1"/>
+      <c r="DR56" s="1"/>
+      <c r="DS56" s="1"/>
+      <c r="DT56" s="1"/>
+      <c r="DU56" s="1"/>
+      <c r="DV56" s="1"/>
+      <c r="DW56" s="1"/>
+      <c r="DX56" s="1"/>
+      <c r="DY56" s="1"/>
+      <c r="DZ56" s="1"/>
+      <c r="EA56" s="1"/>
+      <c r="EB56" s="1"/>
+      <c r="EC56" s="1"/>
+      <c r="ED56" s="1"/>
+      <c r="EE56" s="1"/>
+      <c r="EF56" s="1"/>
+      <c r="EG56" s="1"/>
+      <c r="EH56" s="1"/>
+      <c r="EI56" s="1"/>
+      <c r="EJ56" s="1"/>
+      <c r="EK56" s="1"/>
+      <c r="EL56" s="1"/>
+      <c r="EM56" s="1"/>
+      <c r="EN56" s="1"/>
+      <c r="EO56" s="1"/>
+      <c r="EP56" s="1"/>
+      <c r="EQ56" s="1"/>
+      <c r="ER56" s="1"/>
+      <c r="ES56" s="1"/>
+      <c r="ET56" s="1"/>
+      <c r="EU56" s="1"/>
+      <c r="EV56" s="1"/>
+      <c r="EW56" s="1"/>
+      <c r="EX56" s="1"/>
+      <c r="EY56" s="1"/>
+      <c r="EZ56" s="1"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="12"/>
@@ -1911,7 +2176,7 @@
       <c r="E63" s="12"/>
       <c r="F63" s="12"/>
       <c r="G63" s="12"/>
-      <c r="EZ63" s="8"/>
+      <c r="H63" s="12"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="12"/>
@@ -1921,7 +2186,7 @@
       <c r="E64" s="12"/>
       <c r="F64" s="12"/>
       <c r="G64" s="12"/>
-      <c r="EZ64" s="8"/>
+      <c r="H64" s="12"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="12"/>
@@ -1931,7 +2196,7 @@
       <c r="E65" s="12"/>
       <c r="F65" s="12"/>
       <c r="G65" s="12"/>
-      <c r="EZ65" s="8"/>
+      <c r="H65" s="12"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="12"/>
@@ -1941,7 +2206,7 @@
       <c r="E66" s="12"/>
       <c r="F66" s="12"/>
       <c r="G66" s="12"/>
-      <c r="EZ66" s="8"/>
+      <c r="H66" s="12"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="12"/>
@@ -2001,7 +2266,7 @@
       <c r="E72" s="12"/>
       <c r="F72" s="12"/>
       <c r="G72" s="12"/>
-      <c r="H72" s="12"/>
+      <c r="EZ72" s="8"/>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="12"/>
@@ -2011,7 +2276,7 @@
       <c r="E73" s="12"/>
       <c r="F73" s="12"/>
       <c r="G73" s="12"/>
-      <c r="H73" s="12"/>
+      <c r="EZ73" s="8"/>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="12"/>
@@ -2021,7 +2286,7 @@
       <c r="E74" s="12"/>
       <c r="F74" s="12"/>
       <c r="G74" s="12"/>
-      <c r="H74" s="12"/>
+      <c r="EZ74" s="8"/>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="12"/>
@@ -2031,7 +2296,7 @@
       <c r="E75" s="12"/>
       <c r="F75" s="12"/>
       <c r="G75" s="12"/>
-      <c r="H75" s="12"/>
+      <c r="EZ75" s="8"/>
     </row>
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="12"/>
@@ -10445,6 +10710,96 @@
     </row>
     <row r="917" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A917" s="12"/>
+      <c r="B917" s="12"/>
+      <c r="C917" s="12"/>
+      <c r="D917" s="12"/>
+      <c r="E917" s="12"/>
+      <c r="F917" s="12"/>
+      <c r="G917" s="12"/>
+      <c r="H917" s="12"/>
+    </row>
+    <row r="918" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A918" s="12"/>
+      <c r="B918" s="12"/>
+      <c r="C918" s="12"/>
+      <c r="D918" s="12"/>
+      <c r="E918" s="12"/>
+      <c r="F918" s="12"/>
+      <c r="G918" s="12"/>
+      <c r="H918" s="12"/>
+    </row>
+    <row r="919" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A919" s="12"/>
+      <c r="B919" s="12"/>
+      <c r="C919" s="12"/>
+      <c r="D919" s="12"/>
+      <c r="E919" s="12"/>
+      <c r="F919" s="12"/>
+      <c r="G919" s="12"/>
+      <c r="H919" s="12"/>
+    </row>
+    <row r="920" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A920" s="12"/>
+      <c r="B920" s="12"/>
+      <c r="C920" s="12"/>
+      <c r="D920" s="12"/>
+      <c r="E920" s="12"/>
+      <c r="F920" s="12"/>
+      <c r="G920" s="12"/>
+      <c r="H920" s="12"/>
+    </row>
+    <row r="921" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A921" s="12"/>
+      <c r="B921" s="12"/>
+      <c r="C921" s="12"/>
+      <c r="D921" s="12"/>
+      <c r="E921" s="12"/>
+      <c r="F921" s="12"/>
+      <c r="G921" s="12"/>
+      <c r="H921" s="12"/>
+    </row>
+    <row r="922" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A922" s="12"/>
+      <c r="B922" s="12"/>
+      <c r="C922" s="12"/>
+      <c r="D922" s="12"/>
+      <c r="E922" s="12"/>
+      <c r="F922" s="12"/>
+      <c r="G922" s="12"/>
+      <c r="H922" s="12"/>
+    </row>
+    <row r="923" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A923" s="12"/>
+      <c r="B923" s="12"/>
+      <c r="C923" s="12"/>
+      <c r="D923" s="12"/>
+      <c r="E923" s="12"/>
+      <c r="F923" s="12"/>
+      <c r="G923" s="12"/>
+      <c r="H923" s="12"/>
+    </row>
+    <row r="924" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A924" s="12"/>
+      <c r="B924" s="12"/>
+      <c r="C924" s="12"/>
+      <c r="D924" s="12"/>
+      <c r="E924" s="12"/>
+      <c r="F924" s="12"/>
+      <c r="G924" s="12"/>
+      <c r="H924" s="12"/>
+    </row>
+    <row r="925" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A925" s="12"/>
+      <c r="B925" s="12"/>
+      <c r="C925" s="12"/>
+      <c r="D925" s="12"/>
+      <c r="E925" s="12"/>
+      <c r="F925" s="12"/>
+      <c r="G925" s="12"/>
+      <c r="H925" s="12"/>
+    </row>
+    <row r="926" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A926" s="12"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
@@ -10479,7 +10834,7 @@
     <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="2" customFormat="false" ht="105" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B2" s="31" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>